<commit_message>
Plan de riesgos y junta de estatus
minuta de la junta realizada el 13 de marzo de 2015
</commit_message>
<xml_diff>
--- a/Documentacion/SoftPRESS_PlanDeRiesgos.xlsx
+++ b/Documentacion/SoftPRESS_PlanDeRiesgos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>Aceptado</t>
   </si>
@@ -215,6 +215,15 @@
   </si>
   <si>
     <t>Trabajar más de lo planeado.</t>
+  </si>
+  <si>
+    <t>Retraso con las actividades establecidas por la asistencia al curso de blender.</t>
+  </si>
+  <si>
+    <t>Dedicarle horas extras al proyecto</t>
+  </si>
+  <si>
+    <t>Cumplir con los tiempos establecidos</t>
   </si>
 </sst>
 </file>
@@ -767,43 +776,7 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -1273,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1458,7 +1431,7 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="9">
-        <f t="shared" ref="B6:B20" si="0">B5+1</f>
+        <f t="shared" ref="B6" si="0">B5+1</f>
         <v>3</v>
       </c>
       <c r="C6" s="20">
@@ -1674,20 +1647,39 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="9">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
+      <c r="C12" s="20">
+        <v>42076</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="9">

</xml_diff>